<commit_message>
Automatic update by jenkins
</commit_message>
<xml_diff>
--- a/data/advanced_data_example_v20151104.xlsx
+++ b/data/advanced_data_example_v20151104.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="root_hospital_cities" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>cityName</t>
   </si>
@@ -213,13 +213,31 @@
   </si>
   <si>
     <t>root_hospital</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>latitude in degrees</t>
+  </si>
+  <si>
+    <t>longitude in degrees</t>
+  </si>
+  <si>
+    <t>decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +270,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -289,9 +314,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -637,27 +664,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="3">
+        <v>40.712783999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-74.005941000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>37.151164999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-88.731998000000004</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +891,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -905,113 +948,141 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
       </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
       </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1030,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>